<commit_message>
codigos y datos de prueba de le encuesta de capital social
</commit_message>
<xml_diff>
--- a/ee-code/codes_and_simulated_data.xlsx
+++ b/ee-code/codes_and_simulated_data.xlsx
@@ -29330,8 +29330,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B4F042C639D3B945B74A5373225BEFE3" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="0d9c4422903ad3b390c3065a0889b065">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0b3b6417-da6b-4e3a-993a-9c7c7843b5a8" xmlns:ns3="d0cc75f6-6e6a-4dd6-96f3-ba3b66d1a284" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5cdd1379d3b2ebc3d5165178a79b0b6b" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B4F042C639D3B945B74A5373225BEFE3" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6e27bf83a9d685d5719c0b943bad38d5">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0b3b6417-da6b-4e3a-993a-9c7c7843b5a8" xmlns:ns3="d0cc75f6-6e6a-4dd6-96f3-ba3b66d1a284" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54faafc1f076414c0e717fe56a4513a7" ns2:_="" ns3:_="">
     <xsd:import namespace="0b3b6417-da6b-4e3a-993a-9c7c7843b5a8"/>
     <xsd:import namespace="d0cc75f6-6e6a-4dd6-96f3-ba3b66d1a284"/>
     <xsd:element name="properties">
@@ -29352,6 +29352,7 @@
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -29416,11 +29417,16 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d0cc75f6-6e6a-4dd6-96f3-ba3b66d1a284" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -29439,7 +29445,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -29456,8 +29462,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -29573,7 +29579,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D438E747-1E3F-4372-BF5C-AA967481D319}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45ECF252-756D-45DB-B77B-15C44412057E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>